<commit_message>
binary decimal math, state basted buttons
</commit_message>
<xml_diff>
--- a/diagrams.xlsx
+++ b/diagrams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1770" windowWidth="16155" windowHeight="8280"/>
+    <workbookView xWindow="960" yWindow="1770" windowWidth="15870" windowHeight="5715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Circuit" sheetId="1" r:id="rId1"/>
@@ -647,63 +647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -723,7 +667,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1040,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -1098,12 +1098,12 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="49"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="23" t="s">
@@ -1134,10 +1134,10 @@
       <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="44"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="18"/>
@@ -1164,10 +1164,10 @@
       <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="42"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" spans="1:15">
       <c r="C7" s="5" t="s">
@@ -1192,10 +1192,10 @@
       <c r="K7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="42"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="44"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="52"/>
     </row>
     <row r="8" spans="1:15">
       <c r="C8" s="5" t="s">
@@ -1214,10 +1214,10 @@
       <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="44"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="52"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="27" t="s">
@@ -1243,10 +1243,10 @@
       <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="42"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="52"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="26" t="s">
@@ -1272,10 +1272,10 @@
       <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="44"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1">
       <c r="A11" s="24" t="s">
@@ -1306,10 +1306,10 @@
       <c r="K11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="45"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="47"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="55"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1">
       <c r="A12" s="28" t="s">
@@ -1350,36 +1350,36 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1">
-      <c r="L13" s="48" t="s">
+      <c r="L13" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="50"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="58"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="L14" s="51" t="s">
+      <c r="L14" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1">
-      <c r="D19" s="37">
-        <v>1</v>
-      </c>
-      <c r="E19" s="38"/>
+      <c r="D19" s="42">
+        <v>0</v>
+      </c>
+      <c r="E19" s="43"/>
       <c r="G19">
         <v>7</v>
       </c>
@@ -1400,13 +1400,13 @@
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="44">
+        <v>0</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="44">
         <v>1</v>
-      </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="34">
-        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1414,34 +1414,34 @@
       <c r="H20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="48" t="s">
+      <c r="L20" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="50"/>
+      <c r="M20" s="58"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="C21" s="35"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="35"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="45"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="C22" s="35"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="35"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="45"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1">
-      <c r="C23" s="36"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="36"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="46"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1">
-      <c r="D24" s="37">
-        <v>1</v>
-      </c>
-      <c r="E24" s="38"/>
+      <c r="D24" s="42">
+        <v>0</v>
+      </c>
+      <c r="E24" s="43"/>
       <c r="G24">
         <v>5</v>
       </c>
@@ -1456,12 +1456,12 @@
       <c r="B25">
         <v>4</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="44">
         <v>0</v>
       </c>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="34">
+      <c r="D25" s="36"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="44">
         <v>1</v>
       </c>
       <c r="G25">
@@ -1472,28 +1472,28 @@
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="C26" s="35"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="35"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="C27" s="35"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="35"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="45"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="C28" s="36"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="36"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="46"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="D29" s="53">
+      <c r="D29" s="35">
         <v>1</v>
       </c>
-      <c r="E29" s="53"/>
+      <c r="E29" s="35"/>
       <c r="G29">
         <v>3</v>
       </c>
@@ -1504,7 +1504,7 @@
     <row r="30" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
       <c r="G31" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1519,16 +1519,11 @@
       </c>
       <c r="C32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(D19*(2^G19)+F20*(2^G20)+F25*(2^G25)+D29*(2^G29)+C25*(2^B25)+C20*(2^B20)+D24*(2^G24)+G31*(2^H31)))</f>
-        <v>0xEC</v>
+        <v>0xF</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D25:E28"/>
-    <mergeCell ref="D20:E23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C20:C23"/>
     <mergeCell ref="F20:F23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="C25:C28"/>
@@ -1538,6 +1533,11 @@
     <mergeCell ref="L14:O14"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="L15:O15"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D25:E28"/>
+    <mergeCell ref="D20:E23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C20:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="G31 D19:E19 F20:F23 D24:E24 C20:C23 C25:C28 D29:E29 F25:F28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -1553,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1611,12 +1611,6 @@
       <c r="K2" s="32">
         <v>0.05</v>
       </c>
-      <c r="L2">
-        <v>0.5</v>
-      </c>
-      <c r="M2" s="60">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="2:13">
       <c r="C3" s="31" t="s">
@@ -1637,15 +1631,8 @@
       <c r="J3" s="32">
         <v>1</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="34">
         <v>0.1</v>
-      </c>
-      <c r="L3" s="60">
-        <f>L2*2</f>
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:13">
@@ -1670,13 +1657,6 @@
       <c r="K4" s="32">
         <v>0.25</v>
       </c>
-      <c r="L4" s="32">
-        <f t="shared" ref="K4:L20" si="0">L3*2</f>
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>4</v>
-      </c>
     </row>
     <row r="5" spans="2:13">
       <c r="C5" s="31" t="s">
@@ -1701,12 +1681,8 @@
         <f>K6/2</f>
         <v>0.5</v>
       </c>
-      <c r="L5" s="32">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M5">
-        <v>8</v>
+      <c r="L5">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -1731,12 +1707,12 @@
       <c r="K6" s="32">
         <v>1</v>
       </c>
-      <c r="L6" s="32">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M6">
-        <v>16</v>
+      <c r="L6" s="34">
+        <f>L5*2</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -1745,15 +1721,15 @@
         <v>5</v>
       </c>
       <c r="K7" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K4:L19" si="0">K6*2</f>
         <v>2</v>
       </c>
       <c r="L7" s="32">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>L6*2</f>
+        <v>2</v>
       </c>
       <c r="M7">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1765,11 +1741,11 @@
         <v>4</v>
       </c>
       <c r="L8" s="32">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>L7*2</f>
+        <v>4</v>
       </c>
       <c r="M8">
-        <v>64</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1787,11 +1763,11 @@
         <v>8</v>
       </c>
       <c r="L9" s="32">
-        <f t="shared" si="0"/>
-        <v>64</v>
+        <f>L8*2</f>
+        <v>8</v>
       </c>
       <c r="M9">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -1812,11 +1788,11 @@
         <v>16</v>
       </c>
       <c r="L10" s="32">
-        <f t="shared" si="0"/>
-        <v>128</v>
+        <f>L9*2</f>
+        <v>16</v>
       </c>
       <c r="M10">
-        <v>256</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -1828,11 +1804,11 @@
         <v>32</v>
       </c>
       <c r="L11" s="32">
-        <f t="shared" si="0"/>
-        <v>256</v>
+        <f>L10*2</f>
+        <v>32</v>
       </c>
       <c r="M11">
-        <v>512</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -1862,11 +1838,11 @@
         <v>64</v>
       </c>
       <c r="L12" s="32">
-        <f t="shared" si="0"/>
-        <v>512</v>
+        <f>L11*2</f>
+        <v>64</v>
       </c>
       <c r="M12">
-        <v>1024</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -1896,8 +1872,11 @@
         <v>128</v>
       </c>
       <c r="L13" s="32">
-        <f t="shared" si="0"/>
-        <v>1024</v>
+        <f>L12*2</f>
+        <v>128</v>
+      </c>
+      <c r="M13">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -1927,8 +1906,11 @@
         <v>256</v>
       </c>
       <c r="L14" s="32">
-        <f t="shared" si="0"/>
-        <v>2048</v>
+        <f>L13*2</f>
+        <v>256</v>
+      </c>
+      <c r="M14">
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -1940,8 +1922,11 @@
         <v>512</v>
       </c>
       <c r="L15" s="32">
-        <f t="shared" si="0"/>
-        <v>4096</v>
+        <f>L14*2</f>
+        <v>512</v>
+      </c>
+      <c r="M15">
+        <v>512</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -1953,8 +1938,11 @@
         <v>1024</v>
       </c>
       <c r="L16" s="32">
-        <f t="shared" si="0"/>
-        <v>8192</v>
+        <f>L15*2</f>
+        <v>1024</v>
+      </c>
+      <c r="M16">
+        <v>1024</v>
       </c>
     </row>
     <row r="17" spans="2:12">
@@ -1966,8 +1954,8 @@
         <v>2048</v>
       </c>
       <c r="L17" s="32">
-        <f t="shared" si="0"/>
-        <v>16384</v>
+        <f>L16*2</f>
+        <v>2048</v>
       </c>
     </row>
     <row r="18" spans="2:12">
@@ -1978,7 +1966,10 @@
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
-      <c r="L18" s="32"/>
+      <c r="L18" s="32">
+        <f>L17*2</f>
+        <v>4096</v>
+      </c>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="32" t="s">
@@ -1992,6 +1983,10 @@
       </c>
       <c r="K19" s="32">
         <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="L19" s="32">
+        <f>L18*2</f>
         <v>8192</v>
       </c>
     </row>

</xml_diff>

<commit_message>
timer should work now
</commit_message>
<xml_diff>
--- a/diagrams.xlsx
+++ b/diagrams.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>ra2</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>ct</t>
+  </si>
+  <si>
+    <t>FOSC</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>prescale</t>
+  </si>
+  <si>
+    <t>postscale</t>
   </si>
 </sst>
 </file>
@@ -592,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -649,6 +661,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,63 +735,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1098,12 +1111,12 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="47" t="s">
+      <c r="L4" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="49"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="43"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="23" t="s">
@@ -1134,10 +1147,10 @@
       <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="46"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="18"/>
@@ -1164,10 +1177,10 @@
       <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="50"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="46"/>
     </row>
     <row r="7" spans="1:15">
       <c r="C7" s="5" t="s">
@@ -1192,10 +1205,10 @@
       <c r="K7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="52"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="46"/>
     </row>
     <row r="8" spans="1:15">
       <c r="C8" s="5" t="s">
@@ -1214,10 +1227,10 @@
       <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="50"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="46"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="27" t="s">
@@ -1243,10 +1256,10 @@
       <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="50"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="52"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="46"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="26" t="s">
@@ -1272,10 +1285,10 @@
       <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="50"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="46"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1">
       <c r="A11" s="24" t="s">
@@ -1306,10 +1319,10 @@
       <c r="K11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="53"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="55"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1">
       <c r="A12" s="28" t="s">
@@ -1350,36 +1363,36 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1">
-      <c r="L13" s="56" t="s">
+      <c r="L13" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="58"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1">
-      <c r="D19" s="42">
+      <c r="D19" s="39">
         <v>0</v>
       </c>
-      <c r="E19" s="43"/>
+      <c r="E19" s="40"/>
       <c r="G19">
         <v>7</v>
       </c>
@@ -1400,12 +1413,12 @@
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="36">
         <v>0</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="44">
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="36">
         <v>1</v>
       </c>
       <c r="G20">
@@ -1414,34 +1427,34 @@
       <c r="H20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="56" t="s">
+      <c r="L20" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="58"/>
+      <c r="M20" s="52"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="C21" s="45"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="45"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="C22" s="45"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="45"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1">
-      <c r="C23" s="46"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="46"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1">
-      <c r="D24" s="42">
+      <c r="D24" s="39">
         <v>0</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="40"/>
       <c r="G24">
         <v>5</v>
       </c>
@@ -1456,12 +1469,12 @@
       <c r="B25">
         <v>4</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="36">
         <v>0</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="44">
+      <c r="D25" s="56"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="36">
         <v>1</v>
       </c>
       <c r="G25">
@@ -1472,28 +1485,28 @@
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="C26" s="45"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="45"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="C27" s="45"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="45"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="C28" s="46"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="46"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="D29" s="35">
+      <c r="D29" s="55">
         <v>1</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="55"/>
       <c r="G29">
         <v>3</v>
       </c>
@@ -1524,6 +1537,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D25:E28"/>
+    <mergeCell ref="D20:E23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C20:C23"/>
     <mergeCell ref="F20:F23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="C25:C28"/>
@@ -1533,11 +1551,6 @@
     <mergeCell ref="L14:O14"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="L15:O15"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D25:E28"/>
-    <mergeCell ref="D20:E23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C20:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="G31 D19:E19 F20:F23 D24:E24 C20:C23 C25:C28 D29:E29 F25:F28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -1553,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1708,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="34">
-        <f>L5*2</f>
+        <f t="shared" ref="L6:L19" si="0">L5*2</f>
         <v>1</v>
       </c>
       <c r="M6" s="34">
@@ -1721,11 +1734,11 @@
         <v>5</v>
       </c>
       <c r="K7" s="32">
-        <f t="shared" ref="K4:L19" si="0">K6*2</f>
+        <f t="shared" ref="K7:K19" si="1">K6*2</f>
         <v>2</v>
       </c>
       <c r="L7" s="32">
-        <f>L6*2</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M7">
@@ -1737,11 +1750,11 @@
         <v>6</v>
       </c>
       <c r="K8" s="32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L8" s="32">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L8" s="32">
-        <f>L7*2</f>
         <v>4</v>
       </c>
       <c r="M8">
@@ -1759,11 +1772,11 @@
         <v>7</v>
       </c>
       <c r="K9" s="32">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L9" s="32">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L9" s="32">
-        <f>L8*2</f>
         <v>8</v>
       </c>
       <c r="M9">
@@ -1784,11 +1797,11 @@
         <v>8</v>
       </c>
       <c r="K10" s="32">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L10" s="32">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L10" s="32">
-        <f>L9*2</f>
         <v>16</v>
       </c>
       <c r="M10">
@@ -1800,11 +1813,11 @@
         <v>9</v>
       </c>
       <c r="K11" s="32">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="L11" s="32">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="L11" s="32">
-        <f>L10*2</f>
         <v>32</v>
       </c>
       <c r="M11">
@@ -1834,11 +1847,11 @@
         <v>10</v>
       </c>
       <c r="K12" s="32">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="L12" s="32">
         <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="L12" s="32">
-        <f>L11*2</f>
         <v>64</v>
       </c>
       <c r="M12">
@@ -1868,11 +1881,11 @@
         <v>11</v>
       </c>
       <c r="K13" s="32">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="L13" s="32">
         <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="L13" s="32">
-        <f>L12*2</f>
         <v>128</v>
       </c>
       <c r="M13">
@@ -1902,11 +1915,11 @@
         <v>12</v>
       </c>
       <c r="K14" s="32">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="L14" s="32">
         <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-      <c r="L14" s="32">
-        <f>L13*2</f>
         <v>256</v>
       </c>
       <c r="M14">
@@ -1918,11 +1931,11 @@
         <v>13</v>
       </c>
       <c r="K15" s="32">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="L15" s="32">
         <f t="shared" si="0"/>
-        <v>512</v>
-      </c>
-      <c r="L15" s="32">
-        <f>L14*2</f>
         <v>512</v>
       </c>
       <c r="M15">
@@ -1934,11 +1947,11 @@
         <v>14</v>
       </c>
       <c r="K16" s="32">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="L16" s="32">
         <f t="shared" si="0"/>
-        <v>1024</v>
-      </c>
-      <c r="L16" s="32">
-        <f>L15*2</f>
         <v>1024</v>
       </c>
       <c r="M16">
@@ -1950,11 +1963,11 @@
         <v>15</v>
       </c>
       <c r="K17" s="32">
+        <f t="shared" si="1"/>
+        <v>2048</v>
+      </c>
+      <c r="L17" s="32">
         <f t="shared" si="0"/>
-        <v>2048</v>
-      </c>
-      <c r="L17" s="32">
-        <f>L16*2</f>
         <v>2048</v>
       </c>
     </row>
@@ -1963,11 +1976,11 @@
         <v>16</v>
       </c>
       <c r="K18" s="32">
+        <f t="shared" si="1"/>
+        <v>4096</v>
+      </c>
+      <c r="L18" s="32">
         <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-      <c r="L18" s="32">
-        <f>L17*2</f>
         <v>4096</v>
       </c>
     </row>
@@ -1982,11 +1995,11 @@
         <v>17</v>
       </c>
       <c r="K19" s="32">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="L19" s="32">
         <f t="shared" si="0"/>
-        <v>8192</v>
-      </c>
-      <c r="L19" s="32">
-        <f>L18*2</f>
         <v>8192</v>
       </c>
     </row>
@@ -1997,8 +2010,39 @@
       <c r="C20">
         <v>4</v>
       </c>
+      <c r="F20" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20">
+        <f>8*1000*1000</f>
+        <v>8000000</v>
+      </c>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="E21" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="35">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <f>G20/F21</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="E22" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22">
+        <v>250</v>
+      </c>
+      <c r="G22" s="35">
+        <f>G21/F22</f>
+        <v>2000</v>
+      </c>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="32" t="s">
@@ -2007,6 +2051,16 @@
       <c r="C23">
         <v>3</v>
       </c>
+      <c r="E23" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="35">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <f>G22/F23</f>
+        <v>200</v>
+      </c>
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="32" t="s">
@@ -2022,6 +2076,13 @@
       </c>
       <c r="C25">
         <v>3</v>
+      </c>
+      <c r="G25">
+        <f>1/G23</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:12">

</xml_diff>

<commit_message>
menu state machine works
</commit_message>
<xml_diff>
--- a/diagrams.xlsx
+++ b/diagrams.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
   <si>
     <t>ra2</t>
   </si>
@@ -202,24 +202,12 @@
     <t>auto</t>
   </si>
   <si>
-    <t>\/</t>
-  </si>
-  <si>
-    <t>/\</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
     <t>rep</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>trigger</t>
-  </si>
-  <si>
     <t>hold</t>
   </si>
   <si>
@@ -241,9 +229,6 @@
     <t>adjustr</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
@@ -290,6 +275,42 @@
   </si>
   <si>
     <t>Interrupts</t>
+  </si>
+  <si>
+    <t>"1/10"</t>
+  </si>
+  <si>
+    <t>"1/20"</t>
+  </si>
+  <si>
+    <t>"1/4"</t>
+  </si>
+  <si>
+    <t>"1/2"</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>release-&gt;0</t>
+  </si>
+  <si>
+    <t>fine=128</t>
+  </si>
+  <si>
+    <t>t/e</t>
+  </si>
+  <si>
+    <t>Interrupt</t>
+  </si>
+  <si>
+    <t>countup</t>
+  </si>
+  <si>
+    <t>countdown</t>
+  </si>
+  <si>
+    <t>click</t>
   </si>
 </sst>
 </file>
@@ -610,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -669,6 +690,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,62 +765,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,7 +1087,7 @@
   <dimension ref="A2:O32"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1118,12 +1144,12 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="49" t="s">
+      <c r="L4" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="23" t="s">
@@ -1154,10 +1180,10 @@
       <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="54"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="48"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="18"/>
@@ -1184,10 +1210,10 @@
       <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="54"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
     </row>
     <row r="7" spans="1:15">
       <c r="C7" s="5" t="s">
@@ -1212,10 +1238,10 @@
       <c r="K7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="52"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="54"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="48"/>
     </row>
     <row r="8" spans="1:15">
       <c r="C8" s="5" t="s">
@@ -1234,10 +1260,10 @@
       <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="54"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="48"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="27" t="s">
@@ -1263,10 +1289,10 @@
       <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="52"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="54"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="26" t="s">
@@ -1292,10 +1318,10 @@
       <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="54"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1">
       <c r="A11" s="24" t="s">
@@ -1326,10 +1352,10 @@
       <c r="K11" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="57"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="51"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1">
       <c r="A12" s="28" t="s">
@@ -1370,36 +1396,36 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1">
-      <c r="L13" s="58" t="s">
+      <c r="L13" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="60"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="L14" s="61" t="s">
+      <c r="L14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="62"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1">
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1">
-      <c r="D19" s="44">
-        <v>0</v>
-      </c>
-      <c r="E19" s="45"/>
+      <c r="D19" s="41">
+        <v>1</v>
+      </c>
+      <c r="E19" s="42"/>
       <c r="G19">
         <v>7</v>
       </c>
@@ -1420,48 +1446,47 @@
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="46">
-        <v>0</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="46">
+      <c r="C20" s="38">
         <v>1</v>
       </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="38"/>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="58" t="s">
+      <c r="L20" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="60"/>
+      <c r="M20" s="54"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="C21" s="47"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="47"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="C22" s="47"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="47"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="39"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1">
-      <c r="C23" s="48"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="48"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1">
-      <c r="D24" s="44">
-        <v>0</v>
-      </c>
-      <c r="E24" s="45"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="41">
+        <v>1</v>
+      </c>
+      <c r="E24" s="42"/>
       <c r="G24">
         <v>5</v>
       </c>
@@ -1476,14 +1501,12 @@
       <c r="B25">
         <v>4</v>
       </c>
-      <c r="C25" s="46">
-        <v>0</v>
-      </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="46">
+      <c r="C25" s="38">
         <v>1</v>
       </c>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="38"/>
       <c r="G25">
         <v>2</v>
       </c>
@@ -1492,28 +1515,28 @@
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="C26" s="47"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="47"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="C27" s="47"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="47"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="C28" s="48"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="48"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="D29" s="37">
+      <c r="C28" s="40"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="40"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1">
+      <c r="D29" s="63">
         <v>1</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="64"/>
       <c r="G29">
         <v>3</v>
       </c>
@@ -1524,7 +1547,7 @@
     <row r="30" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
       <c r="G31" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1539,11 +1562,16 @@
       </c>
       <c r="C32" t="str">
         <f>CONCATENATE("0x",DEC2HEX(D19*(2^G19)+F20*(2^G20)+F25*(2^G25)+D29*(2^G29)+C25*(2^B25)+C20*(2^B20)+D24*(2^G24)+G31*(2^H31)))</f>
-        <v>0xF</v>
+        <v>0xF8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D25:E28"/>
+    <mergeCell ref="D20:E23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C20:C23"/>
     <mergeCell ref="F20:F23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="C25:C28"/>
@@ -1553,11 +1581,6 @@
     <mergeCell ref="L14:O14"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="L15:O15"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D25:E28"/>
-    <mergeCell ref="D20:E23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C20:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="G31 D19:E19 F20:F23 D24:E24 C20:C23 C25:C28 D29:E29 F25:F28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -1571,15 +1594,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="37"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="1:18">
       <c r="D1" s="31" t="s">
         <v>53</v>
       </c>
@@ -1595,35 +1622,40 @@
       <c r="H1" s="31" t="s">
         <v>52</v>
       </c>
+      <c r="I1" s="37" t="s">
+        <v>93</v>
+      </c>
       <c r="K1" s="31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13">
-      <c r="B2" s="31"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="B2" s="31">
+        <v>0</v>
+      </c>
       <c r="C2" s="31" t="s">
         <v>55</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>66</v>
+      <c r="E2" s="31">
+        <v>4</v>
+      </c>
+      <c r="F2" s="31">
+        <v>1</v>
+      </c>
+      <c r="G2" s="31">
+        <v>5</v>
+      </c>
+      <c r="H2" s="31">
+        <v>6</v>
       </c>
       <c r="J2" s="31">
         <v>0</v>
@@ -1631,22 +1663,35 @@
       <c r="K2" s="32">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="3" spans="2:13">
+      <c r="N2" s="37">
+        <f t="shared" ref="N2:N5" si="0">K2/60</f>
+        <v>8.3333333333333339E-4</v>
+      </c>
+      <c r="P2">
+        <v>0.05</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0</v>
+      </c>
+      <c r="F3" s="31">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
       </c>
       <c r="J3" s="32">
         <v>1</v>
@@ -1654,22 +1699,39 @@
       <c r="K3" s="34">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="2:13">
+      <c r="N3" s="37">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3">
+        <f>P3/P2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>70</v>
+      <c r="D4" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="31">
+        <v>1</v>
+      </c>
+      <c r="F4" s="31">
+        <v>3</v>
+      </c>
+      <c r="H4" s="31">
+        <v>7</v>
       </c>
       <c r="J4" s="32">
         <v>2</v>
@@ -1677,22 +1739,39 @@
       <c r="K4" s="32">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="2:13">
+      <c r="N4" s="37">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="P4">
+        <v>0.25</v>
+      </c>
+      <c r="Q4" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="R4" s="37">
+        <f t="shared" ref="R4:R21" si="1">P4/P3</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="B5">
+        <v>3</v>
+      </c>
       <c r="C5" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>71</v>
+      <c r="D5" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="31">
+        <v>2</v>
+      </c>
+      <c r="F5" s="31">
+        <v>4</v>
+      </c>
+      <c r="H5" s="31">
+        <v>8</v>
       </c>
       <c r="J5" s="32">
         <v>3</v>
@@ -1704,22 +1783,39 @@
       <c r="L5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="2:13">
+      <c r="N5" s="37">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="R5" s="37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="B6">
+        <v>4</v>
+      </c>
       <c r="C6" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="31" t="s">
+      <c r="D6" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>72</v>
+      <c r="E6" s="31">
+        <v>3</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0</v>
+      </c>
+      <c r="H6" s="31">
+        <v>9</v>
       </c>
       <c r="J6" s="32">
         <v>4</v>
@@ -1728,278 +1824,500 @@
         <v>1</v>
       </c>
       <c r="L6" s="34">
-        <f t="shared" ref="L6:L19" si="0">L5*2</f>
+        <f t="shared" ref="L6:L19" si="2">L5*2</f>
         <v>1</v>
       </c>
       <c r="M6" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:13">
+      <c r="N6">
+        <f>K6/60</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="C7" s="31"/>
       <c r="J7" s="32">
         <v>5</v>
       </c>
       <c r="K7" s="32">
-        <f t="shared" ref="K7:K19" si="1">K6*2</f>
+        <f t="shared" ref="K7:K19" si="3">K6*2</f>
         <v>2</v>
       </c>
       <c r="L7" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:13">
+      <c r="N7" s="37">
+        <f t="shared" ref="N7:N19" si="4">K7/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="J8" s="32">
         <v>6</v>
       </c>
       <c r="K8" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L8" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:13">
-      <c r="C9" s="31" t="s">
-        <v>65</v>
+      <c r="N8" s="37">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="P8">
+        <f>P7*2</f>
+        <v>10</v>
+      </c>
+      <c r="R8" s="37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>96</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="J9" s="32">
         <v>7</v>
       </c>
       <c r="K9" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L9" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="M9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:13">
+      <c r="N9" s="37">
+        <f t="shared" si="4"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="P9">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="B10">
+        <v>6</v>
+      </c>
       <c r="C10" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="31" t="s">
         <v>55</v>
       </c>
+      <c r="I10" s="37" t="s">
+        <v>94</v>
+      </c>
       <c r="J10" s="32">
         <v>8</v>
       </c>
       <c r="K10" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="L10" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:13">
+      <c r="N10" s="37">
+        <f t="shared" si="4"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="P10">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="J11" s="32">
         <v>9</v>
       </c>
       <c r="K11" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L11" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="M11">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="2:13">
+      <c r="N11" s="37">
+        <f t="shared" si="4"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="P11">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
       <c r="C12" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>56</v>
+      <c r="H12" s="31">
+        <v>2</v>
       </c>
       <c r="J12" s="32">
         <v>10</v>
       </c>
       <c r="K12" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="L12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="M12">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="2:13">
+      <c r="N12" s="37">
+        <f t="shared" si="4"/>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="P12">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="37">
+        <f t="shared" ref="Q12:Q23" si="5">P12/60</f>
+        <v>1</v>
+      </c>
+      <c r="R12" s="37">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="B13">
+        <v>8</v>
+      </c>
       <c r="C13" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>76</v>
-      </c>
       <c r="F13" s="33" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="H13" s="31">
+        <v>3</v>
       </c>
       <c r="J13" s="32">
         <v>11</v>
       </c>
       <c r="K13" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="L13" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="M13">
         <v>128</v>
       </c>
-    </row>
-    <row r="14" spans="2:13">
+      <c r="N13" s="37">
+        <f t="shared" si="4"/>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="P13">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="37">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="R13" s="37">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="B14">
+        <v>9</v>
+      </c>
       <c r="C14" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>77</v>
-      </c>
       <c r="G14" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>57</v>
+        <v>73</v>
+      </c>
+      <c r="H14" s="31">
+        <v>4</v>
       </c>
       <c r="J14" s="32">
         <v>12</v>
       </c>
       <c r="K14" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="L14" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="M14">
         <v>256</v>
       </c>
-    </row>
-    <row r="15" spans="2:13">
+      <c r="N14" s="37">
+        <f t="shared" si="4"/>
+        <v>4.2666666666666666</v>
+      </c>
+      <c r="P14">
+        <v>120</v>
+      </c>
+      <c r="Q14" s="37">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R14" s="37">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="J15" s="32">
         <v>13</v>
       </c>
       <c r="K15" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="L15" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>512</v>
       </c>
       <c r="M15">
         <v>512</v>
       </c>
-    </row>
-    <row r="16" spans="2:13">
+      <c r="N15" s="37">
+        <f t="shared" si="4"/>
+        <v>8.5333333333333332</v>
+      </c>
+      <c r="P15">
+        <v>180</v>
+      </c>
+      <c r="Q15" s="37">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="R15" s="37">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>95</v>
+      </c>
       <c r="J16" s="32">
         <v>14</v>
       </c>
       <c r="K16" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
       <c r="L16" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1024</v>
       </c>
       <c r="M16">
         <v>1024</v>
       </c>
-    </row>
-    <row r="17" spans="2:12">
+      <c r="N16" s="37">
+        <f t="shared" si="4"/>
+        <v>17.066666666666666</v>
+      </c>
+      <c r="P16">
+        <v>300</v>
+      </c>
+      <c r="Q16" s="37">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="R16" s="37">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18">
       <c r="J17" s="32">
         <v>15</v>
       </c>
       <c r="K17" s="32">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
+      <c r="L17" s="32">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
+      <c r="N17" s="37">
+        <f t="shared" si="4"/>
+        <v>34.133333333333333</v>
+      </c>
+      <c r="P17">
+        <v>600</v>
+      </c>
+      <c r="Q17" s="37">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="R17" s="37">
         <f t="shared" si="1"/>
-        <v>2048</v>
-      </c>
-      <c r="L17" s="32">
-        <f t="shared" si="0"/>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18">
       <c r="J18" s="32">
         <v>16</v>
       </c>
       <c r="K18" s="32">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+      <c r="L18" s="32">
+        <f t="shared" si="2"/>
+        <v>4096</v>
+      </c>
+      <c r="N18" s="37">
+        <f t="shared" si="4"/>
+        <v>68.266666666666666</v>
+      </c>
+      <c r="P18">
+        <v>1200</v>
+      </c>
+      <c r="Q18" s="37">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="R18" s="37">
         <f t="shared" si="1"/>
-        <v>4096</v>
-      </c>
-      <c r="L18" s="32">
-        <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
       <c r="B19" s="32" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G19">
         <f>4*1000*1000</f>
@@ -2009,23 +2327,38 @@
         <v>17</v>
       </c>
       <c r="K19" s="32">
+        <f t="shared" si="3"/>
+        <v>8192</v>
+      </c>
+      <c r="L19" s="32">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="N19" s="37">
+        <f t="shared" si="4"/>
+        <v>136.53333333333333</v>
+      </c>
+      <c r="P19">
+        <v>1800</v>
+      </c>
+      <c r="Q19" s="37">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="R19" s="37">
         <f t="shared" si="1"/>
-        <v>8192</v>
-      </c>
-      <c r="L19" s="32">
-        <f t="shared" si="0"/>
-        <v>8192</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18">
       <c r="B20" s="32" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G20">
         <f>G19/4</f>
@@ -2033,10 +2366,22 @@
       </c>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
-    </row>
-    <row r="21" spans="2:12">
+      <c r="P20">
+        <f>45*60</f>
+        <v>2700</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="R20" s="37">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18">
       <c r="E21" s="35" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F21" s="35">
         <v>4</v>
@@ -2045,8 +2390,19 @@
         <f>G20/F21</f>
         <v>250000</v>
       </c>
-    </row>
-    <row r="22" spans="2:12">
+      <c r="P21">
+        <v>3600</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="R21" s="37">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18">
       <c r="E22" s="35" t="s">
         <v>58</v>
       </c>
@@ -2057,16 +2413,28 @@
         <f>G21/F22</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="23" spans="2:12">
+      <c r="P22">
+        <f>90*60</f>
+        <v>5400</v>
+      </c>
+      <c r="Q22" s="37">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="R22" s="37">
+        <f t="shared" ref="R22:R23" si="6">P22/P21</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18">
       <c r="B23" s="32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F23" s="35">
         <v>10</v>
@@ -2075,44 +2443,56 @@
         <f>G22/F23</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="2:12">
+      <c r="P23">
+        <f>159*60</f>
+        <v>9540</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>159</v>
+      </c>
+      <c r="R23" s="37">
+        <f t="shared" si="6"/>
+        <v>1.7666666666666666</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18">
       <c r="B24" s="32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:18">
       <c r="B25" s="32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="F25" s="36" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G25">
         <f>1/G23</f>
         <v>0.01</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18">
       <c r="B28" s="32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:18">
       <c r="B29" s="32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C29">
         <v>3</v>

</xml_diff>